<commit_message>
git fix static value
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t/>
+    <t>sn</t>
   </si>
   <si>
     <t>A</t>
@@ -68,58 +68,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>5.0</v>
+      <c r="A2" t="n">
+        <v>1.0</v>
       </c>
-      <c r="B2" t="n" s="0">
+      <c r="B2"/>
+      <c r="C2" t="n">
         <v>3.0</v>
       </c>
-      <c r="C2" t="n" s="0">
-        <v>10.0</v>
-      </c>
+      <c r="D2"/>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="0">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="n">
         <v>7.0</v>
       </c>
-      <c r="B3" t="n" s="0">
+      <c r="C3" t="n">
         <v>8.0</v>
       </c>
-      <c r="C3" t="n" s="0">
+      <c r="D3" t="n">
         <v>15.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="0">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="n">
         <v>9.0</v>
       </c>
-      <c r="B4" t="n" s="0">
+      <c r="C4" t="n">
         <v>9.0</v>
       </c>
-      <c r="C4" t="n" s="0">
-        <v>24.0</v>
-      </c>
+      <c r="D4"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>